<commit_message>
Key based equity data for segmentation.
</commit_message>
<xml_diff>
--- a/data/key_equity.xlsx
+++ b/data/key_equity.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eacon\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tandrewsimpson/transit_segmentation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D48B8CD1-59C0-477F-8E23-CFB07AB5D69A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61B79B3B-D122-0748-8A48-64DE028ED6DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45800" yWindow="-3580" windowWidth="13560" windowHeight="18860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Equity Data by SEPTA Bus Route " sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Equity Data by SEPTA Bus Route '!$A$1:$A$128</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Equity Data by SEPTA Bus Route '!$A$1:$A$131</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -107,7 +107,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="20">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -989,21 +989,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I127"/>
+  <dimension ref="A1:I130"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="11.5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.6640625" style="2" customWidth="1"/>
     <col min="3" max="9" width="10.6640625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="10" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="10" customFormat="1" ht="32">
       <c r="A1" s="7" t="s">
         <v>13</v>
       </c>
@@ -1032,7 +1032,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -1061,7 +1061,7 @@
         <v>1.6992187499999999E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -1090,7 +1090,7 @@
         <v>2.4966560170394E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -1119,7 +1119,7 @@
         <v>3.4188943032297997E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -1148,7 +1148,7 @@
         <v>3.9109706308442002E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -1177,7 +1177,7 @@
         <v>3.7699874333752201E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -1206,7 +1206,7 @@
         <v>2.3059904878961101E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -1235,7 +1235,7 @@
         <v>2.6032925370855699E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -1264,7 +1264,7 @@
         <v>2.45574320277878E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -1293,7 +1293,7 @@
         <v>1.38817159516868E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9">
       <c r="A11" s="4">
         <v>12</v>
       </c>
@@ -1322,7 +1322,7 @@
         <v>1.81902635748236E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9">
       <c r="A12" s="4">
         <v>14</v>
       </c>
@@ -1351,7 +1351,7 @@
         <v>1.6387700855384098E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9">
       <c r="A13" s="4">
         <v>16</v>
       </c>
@@ -1380,7 +1380,7 @@
         <v>4.5463092945055697E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9">
       <c r="A14" s="4">
         <v>17</v>
       </c>
@@ -1409,7 +1409,7 @@
         <v>1.6090835665583499E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9">
       <c r="A15" s="4">
         <v>18</v>
       </c>
@@ -1438,7 +1438,7 @@
         <v>2.2211802664446299E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9">
       <c r="A16" s="4">
         <v>19</v>
       </c>
@@ -1467,7 +1467,7 @@
         <v>2.7150044923629799E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9">
       <c r="A17" s="4">
         <v>20</v>
       </c>
@@ -1496,7 +1496,7 @@
         <v>2.0918825778735901E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9">
       <c r="A18" s="4">
         <v>21</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>2.4851823798541499E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9">
       <c r="A19" s="4">
         <v>22</v>
       </c>
@@ -1554,7 +1554,7 @@
         <v>2.2081311062086401E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9">
       <c r="A20" s="4">
         <v>23</v>
       </c>
@@ -1583,7 +1583,7 @@
         <v>3.1865336111415697E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9">
       <c r="A21" s="4">
         <v>24</v>
       </c>
@@ -1612,7 +1612,7 @@
         <v>1.93862852505579E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9">
       <c r="A22" s="4">
         <v>25</v>
       </c>
@@ -1641,7 +1641,7 @@
         <v>2.3387480125231501E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9">
       <c r="A23" s="4">
         <v>26</v>
       </c>
@@ -1670,7 +1670,7 @@
         <v>2.65207288455344E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9">
       <c r="A24" s="4">
         <v>27</v>
       </c>
@@ -1699,7 +1699,7 @@
         <v>1.0743040685224799E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9">
       <c r="A25" s="4">
         <v>28</v>
       </c>
@@ -1728,7 +1728,7 @@
         <v>2.3577731092437E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9">
       <c r="A26" s="4">
         <v>29</v>
       </c>
@@ -1757,7 +1757,7 @@
         <v>2.61667703795893E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9">
       <c r="A27" s="4">
         <v>30</v>
       </c>
@@ -1786,7 +1786,7 @@
         <v>3.3926545660805399E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9">
       <c r="A28" s="4">
         <v>31</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>3.19084034910238E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9">
       <c r="A29" s="4">
         <v>32</v>
       </c>
@@ -1844,7 +1844,7 @@
         <v>1.76111267877564E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9">
       <c r="A30" s="4">
         <v>33</v>
       </c>
@@ -1873,7 +1873,7 @@
         <v>2.8021721541046901E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9">
       <c r="A31" s="4">
         <v>35</v>
       </c>
@@ -1902,7 +1902,7 @@
         <v>2.15036045314109E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9">
       <c r="A32" s="4">
         <v>37</v>
       </c>
@@ -1931,7 +1931,7 @@
         <v>2.16230721133806E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9">
       <c r="A33" s="4">
         <v>38</v>
       </c>
@@ -1960,7 +1960,7 @@
         <v>2.55599114472835E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9">
       <c r="A34" s="4">
         <v>39</v>
       </c>
@@ -1989,7 +1989,7 @@
         <v>2.9713441451346901E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9">
       <c r="A35" s="4">
         <v>40</v>
       </c>
@@ -2018,7 +2018,7 @@
         <v>2.28638930163447E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9">
       <c r="A36" s="4">
         <v>42</v>
       </c>
@@ -2047,7 +2047,7 @@
         <v>2.1810867919411499E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9">
       <c r="A37" s="4">
         <v>43</v>
       </c>
@@ -2076,7 +2076,7 @@
         <v>2.11187048111183E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9">
       <c r="A38" s="4">
         <v>44</v>
       </c>
@@ -2105,7 +2105,7 @@
         <v>1.41868347628397E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9">
       <c r="A39" s="4">
         <v>45</v>
       </c>
@@ -2134,7 +2134,7 @@
         <v>1.9678018976190901E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9">
       <c r="A40" s="4">
         <v>46</v>
       </c>
@@ -2163,7 +2163,7 @@
         <v>2.1950699320991199E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9">
       <c r="A41" s="4">
         <v>47</v>
       </c>
@@ -2192,7 +2192,7 @@
         <v>2.14204339171476E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9">
       <c r="A42" s="4">
         <v>48</v>
       </c>
@@ -2221,7 +2221,7 @@
         <v>2.2061915491684101E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9">
       <c r="A43" s="4">
         <v>49</v>
       </c>
@@ -2250,7 +2250,7 @@
         <v>1.4347050958252901E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9">
       <c r="A44" s="4">
         <v>50</v>
       </c>
@@ -2279,7 +2279,7 @@
         <v>2.3485837447836298E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9">
       <c r="A45" s="4">
         <v>52</v>
       </c>
@@ -2308,7 +2308,7 @@
         <v>2.99952065616844E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9">
       <c r="A46" s="4">
         <v>53</v>
       </c>
@@ -2337,7 +2337,7 @@
         <v>2.8195383539286599E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9">
       <c r="A47" s="4">
         <v>54</v>
       </c>
@@ -2366,7 +2366,7 @@
         <v>3.9203709356546601E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9">
       <c r="A48" s="4">
         <v>55</v>
       </c>
@@ -2395,7 +2395,7 @@
         <v>1.4892644689552601E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9">
       <c r="A49" s="4">
         <v>56</v>
       </c>
@@ -2424,7 +2424,7 @@
         <v>2.6282252020273199E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9">
       <c r="A50" s="4">
         <v>57</v>
       </c>
@@ -2453,7 +2453,7 @@
         <v>1.86713863342594E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9">
       <c r="A51" s="4">
         <v>58</v>
       </c>
@@ -2482,2212 +2482,2299 @@
         <v>1.9141931902294601E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9">
       <c r="A52" s="4">
+        <v>59</v>
+      </c>
+      <c r="B52" s="5">
+        <v>29229.474381905398</v>
+      </c>
+      <c r="C52" s="6">
+        <v>0.25942586657799699</v>
+      </c>
+      <c r="D52" s="6">
+        <v>0.46790691798670903</v>
+      </c>
+      <c r="E52" s="6">
+        <v>0.26481719999901099</v>
+      </c>
+      <c r="F52" s="6">
+        <v>0.13589523821621899</v>
+      </c>
+      <c r="G52" s="6">
+        <v>0.239267174407649</v>
+      </c>
+      <c r="H52" s="6">
+        <v>0.19739211695040701</v>
+      </c>
+      <c r="I52" s="6">
+        <v>1.9141931902294601E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" s="4">
         <v>60</v>
       </c>
-      <c r="B52" s="5">
+      <c r="B53" s="5">
         <v>25091.692047771001</v>
       </c>
-      <c r="C52" s="6">
+      <c r="C53" s="6">
         <v>0.44300757514700201</v>
       </c>
-      <c r="D52" s="6">
+      <c r="D53" s="6">
         <v>0.19595422038270299</v>
       </c>
-      <c r="E52" s="6">
+      <c r="E53" s="6">
         <v>0.52266292739847897</v>
       </c>
-      <c r="F52" s="6">
+      <c r="F53" s="6">
         <v>0.26711192195601002</v>
       </c>
-      <c r="G52" s="6">
+      <c r="G53" s="6">
         <v>0.46528827800517603</v>
       </c>
-      <c r="H52" s="6">
+      <c r="H53" s="6">
         <v>0.16703129689174701</v>
       </c>
-      <c r="I52" s="6">
+      <c r="I53" s="6">
         <v>3.1007931404072899E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A53" s="4">
+    <row r="54" spans="1:9">
+      <c r="A54" s="4">
         <v>61</v>
       </c>
-      <c r="B53" s="5">
+      <c r="B54" s="5">
         <v>30773.165504553301</v>
       </c>
-      <c r="C53" s="6">
+      <c r="C54" s="6">
         <v>0.37153538566741601</v>
       </c>
-      <c r="D53" s="6">
+      <c r="D54" s="6">
         <v>0.29417258599684598</v>
       </c>
-      <c r="E53" s="6">
+      <c r="E54" s="6">
         <v>0.59786686575414905</v>
       </c>
-      <c r="F53" s="6">
+      <c r="F54" s="6">
         <v>7.7572996638085506E-2</v>
       </c>
-      <c r="G53" s="6">
+      <c r="G54" s="6">
         <v>0.43114853038681999</v>
       </c>
-      <c r="H53" s="6">
+      <c r="H54" s="6">
         <v>0.16753338886948099</v>
       </c>
-      <c r="I53" s="6">
+      <c r="I54" s="6">
         <v>3.2699325504527997E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A54" s="4">
+    <row r="55" spans="1:9">
+      <c r="A55" s="4">
         <v>62</v>
       </c>
-      <c r="B54" s="5">
+      <c r="B55" s="5">
         <v>39307.4035509155</v>
       </c>
-      <c r="C54" s="6">
+      <c r="C55" s="6">
         <v>0.25912749525425999</v>
       </c>
-      <c r="D54" s="6">
+      <c r="D55" s="6">
         <v>0.475590445388824</v>
       </c>
-      <c r="E54" s="6">
+      <c r="E55" s="6">
         <v>0.42245998815552399</v>
       </c>
-      <c r="F54" s="6">
+      <c r="F55" s="6">
         <v>7.2855842279656705E-2</v>
       </c>
-      <c r="G54" s="6">
+      <c r="G55" s="6">
         <v>0.28295252383296798</v>
       </c>
-      <c r="H54" s="6">
+      <c r="H55" s="6">
         <v>0.14296517123536701</v>
       </c>
-      <c r="I54" s="6">
+      <c r="I55" s="6">
         <v>2.08754453573766E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A55" s="4">
+    <row r="56" spans="1:9">
+      <c r="A56" s="4">
         <v>64</v>
       </c>
-      <c r="B55" s="5">
+      <c r="B56" s="5">
         <v>30781.3925096985</v>
       </c>
-      <c r="C55" s="6">
+      <c r="C56" s="6">
         <v>0.33411768262416502</v>
       </c>
-      <c r="D55" s="6">
+      <c r="D56" s="6">
         <v>0.31624924237044899</v>
       </c>
-      <c r="E55" s="6">
+      <c r="E56" s="6">
         <v>0.57654299911589602</v>
       </c>
-      <c r="F55" s="6">
+      <c r="F56" s="6">
         <v>6.5131210954517196E-2</v>
       </c>
-      <c r="G55" s="6">
+      <c r="G56" s="6">
         <v>0.46289393388516997</v>
       </c>
-      <c r="H55" s="6">
+      <c r="H56" s="6">
         <v>0.210498812351544</v>
       </c>
-      <c r="I55" s="6">
+      <c r="I56" s="6">
         <v>3.1686460807601E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A56" s="4">
+    <row r="57" spans="1:9">
+      <c r="A57" s="4">
         <v>65</v>
       </c>
-      <c r="B56" s="5">
+      <c r="B57" s="5">
         <v>30987.393022399901</v>
       </c>
-      <c r="C56" s="6">
+      <c r="C57" s="6">
         <v>0.29209790060128699</v>
       </c>
-      <c r="D56" s="6">
+      <c r="D57" s="6">
         <v>0.19647042806999299</v>
       </c>
-      <c r="E56" s="6">
+      <c r="E57" s="6">
         <v>0.72050807030681896</v>
       </c>
-      <c r="F56" s="6">
+      <c r="F57" s="6">
         <v>5.97423596388773E-2</v>
       </c>
-      <c r="G56" s="6">
+      <c r="G57" s="6">
         <v>0.332678845883847</v>
       </c>
-      <c r="H56" s="6">
+      <c r="H57" s="6">
         <v>0.12823430147655401</v>
       </c>
-      <c r="I56" s="6">
+      <c r="I57" s="6">
         <v>1.8690248255719601E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A57" s="4">
+    <row r="58" spans="1:9">
+      <c r="A58" s="4">
+        <v>66</v>
+      </c>
+      <c r="B58" s="5">
+        <v>29229.474381905398</v>
+      </c>
+      <c r="C58" s="6">
+        <v>0.25942586657799699</v>
+      </c>
+      <c r="D58" s="6">
+        <v>0.46790691798670903</v>
+      </c>
+      <c r="E58" s="6">
+        <v>0.26481719999901099</v>
+      </c>
+      <c r="F58" s="6">
+        <v>0.13589523821621899</v>
+      </c>
+      <c r="G58" s="6">
+        <v>0.239267174407649</v>
+      </c>
+      <c r="H58" s="6">
+        <v>0.19739211695040701</v>
+      </c>
+      <c r="I58" s="6">
+        <v>1.9141931902294601E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="A59" s="4">
         <v>67</v>
       </c>
-      <c r="B57" s="5">
+      <c r="B59" s="5">
         <v>31103.340567089199</v>
       </c>
-      <c r="C57" s="6">
+      <c r="C59" s="6">
         <v>0.24415280394375999</v>
       </c>
-      <c r="D57" s="6">
+      <c r="D59" s="6">
         <v>0.39806180590821399</v>
       </c>
-      <c r="E57" s="6">
+      <c r="E59" s="6">
         <v>0.35063768161380099</v>
       </c>
-      <c r="F57" s="6">
+      <c r="F59" s="6">
         <v>0.158050827019521</v>
       </c>
-      <c r="G57" s="6">
+      <c r="G59" s="6">
         <v>0.24380729875231699</v>
       </c>
-      <c r="H57" s="6">
+      <c r="H59" s="6">
         <v>0.100349619004931</v>
       </c>
-      <c r="I57" s="6">
+      <c r="I59" s="6">
         <v>1.94051354293398E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A58" s="4">
+    <row r="60" spans="1:9">
+      <c r="A60" s="4">
         <v>68</v>
       </c>
-      <c r="B58" s="5">
+      <c r="B60" s="5">
         <v>26524.475557616101</v>
       </c>
-      <c r="C58" s="6">
+      <c r="C60" s="6">
         <v>0.33405992248244498</v>
       </c>
-      <c r="D58" s="6">
+      <c r="D60" s="6">
         <v>0.21400551465251999</v>
       </c>
-      <c r="E58" s="6">
+      <c r="E60" s="6">
         <v>0.63632828609763703</v>
       </c>
-      <c r="F58" s="6">
+      <c r="F60" s="6">
         <v>8.0870853148699406E-2</v>
       </c>
-      <c r="G58" s="6">
+      <c r="G60" s="6">
         <v>0.411990231490173</v>
       </c>
-      <c r="H58" s="6">
+      <c r="H60" s="6">
         <v>5.4477585122630498E-2</v>
       </c>
-      <c r="I58" s="6">
+      <c r="I60" s="6">
         <v>1.0395292426556501E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A59" s="4">
+    <row r="61" spans="1:9">
+      <c r="A61" s="4">
         <v>70</v>
       </c>
-      <c r="B59" s="5">
+      <c r="B61" s="5">
         <v>29414.265890546802</v>
       </c>
-      <c r="C59" s="6">
+      <c r="C61" s="6">
         <v>0.270623368714205</v>
       </c>
-      <c r="D59" s="6">
+      <c r="D61" s="6">
         <v>0.34428033929718299</v>
       </c>
-      <c r="E59" s="6">
+      <c r="E61" s="6">
         <v>0.42306727648133602</v>
       </c>
-      <c r="F59" s="6">
+      <c r="F61" s="6">
         <v>0.14899532676482299</v>
       </c>
-      <c r="G59" s="6">
+      <c r="G61" s="6">
         <v>0.268105231564572</v>
       </c>
-      <c r="H59" s="6">
+      <c r="H61" s="6">
         <v>0.13980655932960401</v>
       </c>
-      <c r="I59" s="6">
+      <c r="I61" s="6">
         <v>1.9873237339685601E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A60" s="4">
+    <row r="62" spans="1:9">
+      <c r="A62" s="4">
         <v>73</v>
       </c>
-      <c r="B60" s="5">
+      <c r="B62" s="5">
         <v>30122.7095933413</v>
       </c>
-      <c r="C60" s="6">
+      <c r="C62" s="6">
         <v>0.32232449981192102</v>
       </c>
-      <c r="D60" s="6">
+      <c r="D62" s="6">
         <v>0.506784430854478</v>
       </c>
-      <c r="E60" s="6">
+      <c r="E62" s="6">
         <v>0.313091708263114</v>
       </c>
-      <c r="F60" s="6">
+      <c r="F62" s="6">
         <v>0.15882838617596101</v>
       </c>
-      <c r="G60" s="6">
+      <c r="G62" s="6">
         <v>0.32460365582719303</v>
       </c>
-      <c r="H60" s="6">
+      <c r="H62" s="6">
         <v>0.1249336492891</v>
       </c>
-      <c r="I60" s="6">
+      <c r="I62" s="6">
         <v>1.9447867298578201E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A61" s="4">
+    <row r="63" spans="1:9">
+      <c r="A63" s="4">
+        <v>75</v>
+      </c>
+      <c r="B63" s="5">
+        <v>24303.769836578402</v>
+      </c>
+      <c r="C63" s="6">
+        <v>0.45287635394213799</v>
+      </c>
+      <c r="D63" s="6">
+        <v>0.14213104353922101</v>
+      </c>
+      <c r="E63" s="6">
+        <v>0.67426043590933904</v>
+      </c>
+      <c r="F63" s="6">
+        <v>0.17263067793999901</v>
+      </c>
+      <c r="G63" s="6">
+        <v>0.489576158569835</v>
+      </c>
+      <c r="H63" s="6">
+        <v>0.186064229550646</v>
+      </c>
+      <c r="I63" s="6">
+        <v>3.9203709356546601E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="A64" s="4">
         <v>77</v>
       </c>
-      <c r="B61" s="5">
+      <c r="B64" s="5">
         <v>30237.620904309599</v>
       </c>
-      <c r="C61" s="6">
+      <c r="C64" s="6">
         <v>0.25285153226437901</v>
       </c>
-      <c r="D61" s="6">
+      <c r="D64" s="6">
         <v>0.34673334458496602</v>
       </c>
-      <c r="E61" s="6">
+      <c r="E64" s="6">
         <v>0.414373071755119</v>
       </c>
-      <c r="F61" s="6">
+      <c r="F64" s="6">
         <v>0.13943776299732499</v>
       </c>
-      <c r="G61" s="6">
+      <c r="G64" s="6">
         <v>0.249842587812179</v>
       </c>
-      <c r="H61" s="6">
+      <c r="H64" s="6">
         <v>0.189078254326561</v>
       </c>
-      <c r="I61" s="6">
+      <c r="I64" s="6">
         <v>2.2802859292701299E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A62" s="4">
+    <row r="65" spans="1:9">
+      <c r="A65" s="4">
         <v>78</v>
       </c>
-      <c r="B62" s="5">
+      <c r="B65" s="5">
         <v>37183.080041678797</v>
       </c>
-      <c r="C62" s="6">
+      <c r="C65" s="6">
         <v>0.24641525343288301</v>
       </c>
-      <c r="D62" s="6">
+      <c r="D65" s="6">
         <v>0.55998347926597303</v>
       </c>
-      <c r="E62" s="6">
+      <c r="E65" s="6">
         <v>0.232170369828825</v>
       </c>
-      <c r="F62" s="6">
+      <c r="F65" s="6">
         <v>0.10910725954047901</v>
       </c>
-      <c r="G62" s="6">
+      <c r="G65" s="6">
         <v>0.34381295565472297</v>
       </c>
-      <c r="H62" s="6">
+      <c r="H65" s="6">
         <v>1.59007832898172E-2</v>
       </c>
-      <c r="I62" s="6">
+      <c r="I65" s="6">
         <v>6.8146214099216703E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A63" s="4">
+    <row r="66" spans="1:9">
+      <c r="A66" s="4">
         <v>79</v>
       </c>
-      <c r="B63" s="5">
+      <c r="B66" s="5">
         <v>28766.322272889101</v>
       </c>
-      <c r="C63" s="6">
+      <c r="C66" s="6">
         <v>0.321084922948352</v>
       </c>
-      <c r="D63" s="6">
+      <c r="D66" s="6">
         <v>0.44040323080534099</v>
       </c>
-      <c r="E63" s="6">
+      <c r="E66" s="6">
         <v>0.37763529662945999</v>
       </c>
-      <c r="F63" s="6">
+      <c r="F66" s="6">
         <v>0.103534004624416</v>
       </c>
-      <c r="G63" s="6">
+      <c r="G66" s="6">
         <v>0.41544844858347701</v>
       </c>
-      <c r="H63" s="6">
+      <c r="H66" s="6">
         <v>0.191795400540791</v>
       </c>
-      <c r="I63" s="6">
+      <c r="I66" s="6">
         <v>2.30254281266217E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A64" s="4">
+    <row r="67" spans="1:9">
+      <c r="A67" s="4">
         <v>80</v>
       </c>
-      <c r="B64" s="5">
+      <c r="B67" s="5">
         <v>28333.0125663414</v>
       </c>
-      <c r="C64" s="6">
+      <c r="C67" s="6">
         <v>0.32949534310343898</v>
       </c>
-      <c r="D64" s="6">
+      <c r="D67" s="6">
         <v>0.16847731456357501</v>
       </c>
-      <c r="E64" s="6">
+      <c r="E67" s="6">
         <v>0.72204973032522402</v>
       </c>
-      <c r="F64" s="6">
+      <c r="F67" s="6">
         <v>8.03519221653827E-2</v>
       </c>
-      <c r="G64" s="6">
+      <c r="G67" s="6">
         <v>0.39646442258910097</v>
       </c>
-      <c r="H64" s="6">
+      <c r="H67" s="6">
         <v>4.1934106162294101E-2</v>
       </c>
-      <c r="I64" s="6">
+      <c r="I67" s="6">
         <v>1.00854179377669E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A65" s="4">
+    <row r="68" spans="1:9">
+      <c r="A68" s="4">
         <v>84</v>
       </c>
-      <c r="B65" s="5">
+      <c r="B68" s="5">
         <v>30939.061272652401</v>
       </c>
-      <c r="C65" s="6">
+      <c r="C68" s="6">
         <v>0.27310788737181502</v>
       </c>
-      <c r="D65" s="6">
+      <c r="D68" s="6">
         <v>0.48388307734817698</v>
       </c>
-      <c r="E65" s="6">
+      <c r="E68" s="6">
         <v>0.31829220556162802</v>
       </c>
-      <c r="F65" s="6">
+      <c r="F68" s="6">
         <v>0.14096721302969201</v>
       </c>
-      <c r="G65" s="6">
+      <c r="G68" s="6">
         <v>0.253359169783826</v>
       </c>
-      <c r="H65" s="6">
+      <c r="H68" s="6">
         <v>0.120805982215036</v>
       </c>
-      <c r="I65" s="6">
+      <c r="I68" s="6">
         <v>2.4522231204527099E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A66" s="4">
+    <row r="69" spans="1:9">
+      <c r="A69" s="4">
         <v>88</v>
       </c>
-      <c r="B66" s="5">
+      <c r="B69" s="5">
         <v>30237.072399005301</v>
       </c>
-      <c r="C66" s="6">
+      <c r="C69" s="6">
         <v>0.24039304220271501</v>
       </c>
-      <c r="D66" s="6">
+      <c r="D69" s="6">
         <v>0.50101044081372903</v>
       </c>
-      <c r="E66" s="6">
+      <c r="E69" s="6">
         <v>0.25592580444704799</v>
       </c>
-      <c r="F66" s="6">
+      <c r="F69" s="6">
         <v>0.13844602747577101</v>
       </c>
-      <c r="G66" s="6">
+      <c r="G69" s="6">
         <v>0.19871470695384699</v>
       </c>
-      <c r="H66" s="6">
+      <c r="H69" s="6">
         <v>0.143021770682148</v>
       </c>
-      <c r="I66" s="6">
+      <c r="I69" s="6">
         <v>1.41843251088534E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A67" s="4">
+    <row r="70" spans="1:9">
+      <c r="A70" s="4">
         <v>89</v>
       </c>
-      <c r="B67" s="5">
+      <c r="B70" s="5">
         <v>26977.058859597299</v>
       </c>
-      <c r="C67" s="6">
+      <c r="C70" s="6">
         <v>0.41779194924372798</v>
       </c>
-      <c r="D67" s="6">
+      <c r="D70" s="6">
         <v>0.30424520278865402</v>
       </c>
-      <c r="E67" s="6">
+      <c r="E70" s="6">
         <v>0.34129361202192599</v>
       </c>
-      <c r="F67" s="6">
+      <c r="F70" s="6">
         <v>0.33799640924173802</v>
       </c>
-      <c r="G67" s="6">
+      <c r="G70" s="6">
         <v>0.41234832785105302</v>
       </c>
-      <c r="H67" s="6">
+      <c r="H70" s="6">
         <v>0.225419105741686</v>
       </c>
-      <c r="I67" s="6">
+      <c r="I70" s="6">
         <v>4.1247976086685803E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A68" s="4">
+    <row r="71" spans="1:9">
+      <c r="A71" s="4">
         <v>90</v>
       </c>
-      <c r="B68" s="5">
+      <c r="B71" s="5">
         <v>30177.356600709201</v>
       </c>
-      <c r="C68" s="6">
+      <c r="C71" s="6">
         <v>0.29757064135496902</v>
       </c>
-      <c r="D68" s="6">
+      <c r="D71" s="6">
         <v>0.19718584665571601</v>
       </c>
-      <c r="E68" s="6">
+      <c r="E71" s="6">
         <v>0.71686387881485603</v>
       </c>
-      <c r="F68" s="6">
+      <c r="F71" s="6">
         <v>6.3073694133781194E-2</v>
       </c>
-      <c r="G68" s="6">
+      <c r="G71" s="6">
         <v>0.36044534229781899</v>
       </c>
-      <c r="H68" s="6">
+      <c r="H71" s="6">
         <v>8.73234200743494E-2</v>
       </c>
-      <c r="I68" s="6">
+      <c r="I71" s="6">
         <v>1.3475836431226801E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A69" s="4">
+    <row r="72" spans="1:9">
+      <c r="A72" s="4">
         <v>91</v>
       </c>
-      <c r="B69" s="5">
+      <c r="B72" s="5">
         <v>26419.665713798699</v>
       </c>
-      <c r="C69" s="6">
+      <c r="C72" s="6">
         <v>0.38592980118343001</v>
       </c>
-      <c r="D69" s="6">
+      <c r="D72" s="6">
         <v>0.13389147827985301</v>
       </c>
-      <c r="E69" s="6">
+      <c r="E72" s="6">
         <v>0.80336943003820005</v>
       </c>
-      <c r="F69" s="6">
+      <c r="F72" s="6">
         <v>5.8494745383335399E-2</v>
       </c>
-      <c r="G69" s="6">
+      <c r="G72" s="6">
         <v>0.46041738742577099</v>
       </c>
-      <c r="H69" s="6">
+      <c r="H72" s="6">
         <v>0.133846153846154</v>
       </c>
-      <c r="I69" s="6">
+      <c r="I72" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A70" s="4">
+    <row r="73" spans="1:9">
+      <c r="A73" s="4">
         <v>92</v>
       </c>
-      <c r="B70" s="5">
+      <c r="B73" s="5">
         <v>28184.944507809501</v>
       </c>
-      <c r="C70" s="6">
+      <c r="C73" s="6">
         <v>0.34943337500765198</v>
       </c>
-      <c r="D70" s="6">
+      <c r="D73" s="6">
         <v>0.19406415574248001</v>
       </c>
-      <c r="E70" s="6">
+      <c r="E73" s="6">
         <v>0.70086540287898103</v>
       </c>
-      <c r="F70" s="6">
+      <c r="F73" s="6">
         <v>7.7422585654009293E-2</v>
       </c>
-      <c r="G70" s="6">
+      <c r="G73" s="6">
         <v>0.43270740124812501</v>
       </c>
-      <c r="H70" s="6">
+      <c r="H73" s="6">
         <v>4.4779411764705901E-2</v>
       </c>
-      <c r="I70" s="6">
+      <c r="I73" s="6">
         <v>3.5539215686274501E-3</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A71" s="4">
+    <row r="74" spans="1:9">
+      <c r="A74" s="4">
         <v>93</v>
       </c>
-      <c r="B71" s="5">
+      <c r="B74" s="5">
         <v>29122.2365391085</v>
       </c>
-      <c r="C71" s="6">
+      <c r="C74" s="6">
         <v>0.34597575977719103</v>
       </c>
-      <c r="D71" s="6">
+      <c r="D74" s="6">
         <v>0.23812395801471101</v>
       </c>
-      <c r="E71" s="6">
+      <c r="E74" s="6">
         <v>0.63494611862380901</v>
       </c>
-      <c r="F71" s="6">
+      <c r="F74" s="6">
         <v>9.6262044390196505E-2</v>
       </c>
-      <c r="G71" s="6">
+      <c r="G74" s="6">
         <v>0.42039085945640398</v>
       </c>
-      <c r="H71" s="6">
+      <c r="H74" s="6">
         <v>6.1720475785896303E-2</v>
       </c>
-      <c r="I71" s="6">
+      <c r="I74" s="6">
         <v>2.9566694987255698E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A72" s="4">
+    <row r="75" spans="1:9">
+      <c r="A75" s="4">
         <v>94</v>
       </c>
-      <c r="B72" s="5">
+      <c r="B75" s="5">
         <v>28523.7542805392</v>
       </c>
-      <c r="C72" s="6">
+      <c r="C75" s="6">
         <v>0.24673505999987799</v>
       </c>
-      <c r="D72" s="6">
+      <c r="D75" s="6">
         <v>0.32911043061627498</v>
       </c>
-      <c r="E72" s="6">
+      <c r="E75" s="6">
         <v>0.53928947213428902</v>
       </c>
-      <c r="F72" s="6">
+      <c r="F75" s="6">
         <v>7.6779978526789305E-2</v>
       </c>
-      <c r="G72" s="6">
+      <c r="G75" s="6">
         <v>0.28026855626666197</v>
       </c>
-      <c r="H72" s="6">
+      <c r="H75" s="6">
         <v>7.7719298245613994E-2</v>
       </c>
-      <c r="I72" s="6">
+      <c r="I75" s="6">
         <v>1.5614035087719301E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A73" s="4">
+    <row r="76" spans="1:9">
+      <c r="A76" s="4">
         <v>95</v>
       </c>
-      <c r="B73" s="5">
+      <c r="B76" s="5">
         <v>28746.499466809601</v>
       </c>
-      <c r="C73" s="6">
+      <c r="C76" s="6">
         <v>0.32630751357155802</v>
       </c>
-      <c r="D73" s="6">
+      <c r="D76" s="6">
         <v>0.18482279917862299</v>
       </c>
-      <c r="E73" s="6">
+      <c r="E76" s="6">
         <v>0.71363277837760397</v>
       </c>
-      <c r="F73" s="6">
+      <c r="F76" s="6">
         <v>7.0488736732639098E-2</v>
       </c>
-      <c r="G73" s="6">
+      <c r="G76" s="6">
         <v>0.407981010638365</v>
       </c>
-      <c r="H73" s="6">
+      <c r="H76" s="6">
         <v>3.80703012912482E-2</v>
       </c>
-      <c r="I73" s="6">
+      <c r="I76" s="6">
         <v>9.0494978479196495E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A74" s="4">
+    <row r="77" spans="1:9">
+      <c r="A77" s="4">
         <v>96</v>
       </c>
-      <c r="B74" s="5">
+      <c r="B77" s="5">
         <v>27890.921020506201</v>
       </c>
-      <c r="C74" s="6">
+      <c r="C77" s="6">
         <v>0.356132969382846</v>
       </c>
-      <c r="D74" s="6">
+      <c r="D77" s="6">
         <v>0.19910441552521899</v>
       </c>
-      <c r="E74" s="6">
+      <c r="E77" s="6">
         <v>0.68988068964584903</v>
       </c>
-      <c r="F74" s="6">
+      <c r="F77" s="6">
         <v>8.1815078302118802E-2</v>
       </c>
-      <c r="G74" s="6">
+      <c r="G77" s="6">
         <v>0.431005629948368</v>
       </c>
-      <c r="H74" s="6">
+      <c r="H77" s="6">
         <v>8.4669030732860501E-2</v>
       </c>
-      <c r="I74" s="6">
+      <c r="I77" s="6">
         <v>1.9881796690307301E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A75" s="4">
+    <row r="78" spans="1:9">
+      <c r="A78" s="4">
         <v>97</v>
       </c>
-      <c r="B75" s="5">
+      <c r="B78" s="5">
         <v>31024.046592463401</v>
       </c>
-      <c r="C75" s="6">
+      <c r="C78" s="6">
         <v>0.288139269839296</v>
       </c>
-      <c r="D75" s="6">
+      <c r="D78" s="6">
         <v>0.22149972726405701</v>
       </c>
-      <c r="E75" s="6">
+      <c r="E78" s="6">
         <v>0.69002482061954895</v>
       </c>
-      <c r="F75" s="6">
+      <c r="F78" s="6">
         <v>6.0737275748097203E-2</v>
       </c>
-      <c r="G75" s="6">
+      <c r="G78" s="6">
         <v>0.35650632837165702</v>
       </c>
-      <c r="H75" s="6">
+      <c r="H78" s="6">
         <v>4.5529306220095697E-2</v>
       </c>
-      <c r="I75" s="6">
+      <c r="I78" s="6">
         <v>1.5870215311004798E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A76" s="4">
+    <row r="79" spans="1:9">
+      <c r="A79" s="4">
         <v>98</v>
       </c>
-      <c r="B76" s="5">
+      <c r="B79" s="5">
         <v>30542.649421147798</v>
       </c>
-      <c r="C76" s="6">
+      <c r="C79" s="6">
         <v>0.30118755059998098</v>
       </c>
-      <c r="D76" s="6">
+      <c r="D79" s="6">
         <v>0.20247303076699699</v>
       </c>
-      <c r="E76" s="6">
+      <c r="E79" s="6">
         <v>0.71120387631155102</v>
       </c>
-      <c r="F76" s="6">
+      <c r="F79" s="6">
         <v>6.2273464326089302E-2</v>
       </c>
-      <c r="G76" s="6">
+      <c r="G79" s="6">
         <v>0.36624603652062099</v>
       </c>
-      <c r="H76" s="6">
+      <c r="H79" s="6">
         <v>6.8524868443388204E-2</v>
       </c>
-      <c r="I76" s="6">
+      <c r="I79" s="6">
         <v>1.21099983024953E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A77" s="4">
+    <row r="80" spans="1:9">
+      <c r="A80" s="4">
         <v>99</v>
       </c>
-      <c r="B77" s="5">
+      <c r="B80" s="5">
         <v>28468.5385433624</v>
       </c>
-      <c r="C77" s="6">
+      <c r="C80" s="6">
         <v>0.360907662549387</v>
       </c>
-      <c r="D77" s="6">
+      <c r="D80" s="6">
         <v>0.208930543930647</v>
       </c>
-      <c r="E77" s="6">
+      <c r="E80" s="6">
         <v>0.67989549937125504</v>
       </c>
-      <c r="F77" s="6">
+      <c r="F80" s="6">
         <v>8.4221191998369194E-2</v>
       </c>
-      <c r="G77" s="6">
+      <c r="G80" s="6">
         <v>0.43146302036347101</v>
       </c>
-      <c r="H77" s="6">
+      <c r="H80" s="6">
         <v>5.1533885152612501E-2</v>
       </c>
-      <c r="I77" s="6">
+      <c r="I80" s="6">
         <v>1.3277289187790999E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A78" s="4">
+    <row r="81" spans="1:9">
+      <c r="A81" s="4">
         <v>103</v>
       </c>
-      <c r="B78" s="5">
+      <c r="B81" s="5">
         <v>27416.728537706302</v>
       </c>
-      <c r="C78" s="6">
+      <c r="C81" s="6">
         <v>0.26343551968201301</v>
       </c>
-      <c r="D78" s="6">
+      <c r="D81" s="6">
         <v>0.125247352397589</v>
       </c>
-      <c r="E78" s="6">
+      <c r="E81" s="6">
         <v>0.78951995810253806</v>
       </c>
-      <c r="F78" s="6">
+      <c r="F81" s="6">
         <v>6.8213321786014997E-2</v>
       </c>
-      <c r="G78" s="6">
+      <c r="G81" s="6">
         <v>0.317524837387968</v>
       </c>
-      <c r="H78" s="6">
+      <c r="H81" s="6">
         <v>0.103323634012286</v>
       </c>
-      <c r="I78" s="6">
+      <c r="I81" s="6">
         <v>1.16262528289686E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A79" s="4">
+    <row r="82" spans="1:9">
+      <c r="A82" s="4">
         <v>104</v>
       </c>
-      <c r="B79" s="5">
+      <c r="B82" s="5">
         <v>27388.524209527899</v>
       </c>
-      <c r="C79" s="6">
+      <c r="C82" s="6">
         <v>0.35815918356801901</v>
       </c>
-      <c r="D79" s="6">
+      <c r="D82" s="6">
         <v>0.19035339680557301</v>
       </c>
-      <c r="E79" s="6">
+      <c r="E82" s="6">
         <v>0.69669974260191503</v>
       </c>
-      <c r="F79" s="6">
+      <c r="F82" s="6">
         <v>7.8104675675451998E-2</v>
       </c>
-      <c r="G79" s="6">
+      <c r="G82" s="6">
         <v>0.44236749651424301</v>
       </c>
-      <c r="H79" s="6">
+      <c r="H82" s="6">
         <v>5.5123825285182303E-2</v>
       </c>
-      <c r="I79" s="6">
+      <c r="I82" s="6">
         <v>8.2788580885395108E-3</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A80" s="4">
+    <row r="83" spans="1:9">
+      <c r="A83" s="4">
         <v>105</v>
       </c>
-      <c r="B80" s="5">
+      <c r="B83" s="5">
         <v>28054.634922606601</v>
       </c>
-      <c r="C80" s="6">
+      <c r="C83" s="6">
         <v>0.32405617512798501</v>
       </c>
-      <c r="D80" s="6">
+      <c r="D83" s="6">
         <v>0.12671026376377201</v>
       </c>
-      <c r="E80" s="6">
+      <c r="E83" s="6">
         <v>0.79960102853533899</v>
       </c>
-      <c r="F80" s="6">
+      <c r="F83" s="6">
         <v>5.6705749622949601E-2</v>
       </c>
-      <c r="G80" s="6">
+      <c r="G83" s="6">
         <v>0.38742630974012299</v>
       </c>
-      <c r="H80" s="6">
+      <c r="H83" s="6">
         <v>0.114663730306624</v>
       </c>
-      <c r="I80" s="6">
+      <c r="I83" s="6">
         <v>2.0780958834490899E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A81" s="4">
+    <row r="84" spans="1:9">
+      <c r="A84" s="4">
         <v>106</v>
       </c>
-      <c r="B81" s="5">
+      <c r="B84" s="5">
         <v>27243.961179934398</v>
       </c>
-      <c r="C81" s="6">
+      <c r="C84" s="6">
         <v>0.31006996908432699</v>
       </c>
-      <c r="D81" s="6">
+      <c r="D84" s="6">
         <v>0.13184887761619299</v>
       </c>
-      <c r="E81" s="6">
+      <c r="E84" s="6">
         <v>0.78262785091430498</v>
       </c>
-      <c r="F81" s="6">
+      <c r="F84" s="6">
         <v>6.7270914957934899E-2</v>
       </c>
-      <c r="G81" s="6">
+      <c r="G84" s="6">
         <v>0.36676018693908802</v>
       </c>
-      <c r="H81" s="6">
+      <c r="H84" s="6">
         <v>0.10857663402414</v>
       </c>
-      <c r="I81" s="6">
+      <c r="I84" s="6">
         <v>1.1491687542700999E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A82" s="4">
+    <row r="85" spans="1:9">
+      <c r="A85" s="4">
         <v>107</v>
       </c>
-      <c r="B82" s="5">
+      <c r="B85" s="5">
         <v>26549.404301590999</v>
       </c>
-      <c r="C82" s="6">
+      <c r="C85" s="6">
         <v>0.369132855359523</v>
       </c>
-      <c r="D82" s="6">
+      <c r="D85" s="6">
         <v>0.171163646103874</v>
       </c>
-      <c r="E82" s="6">
+      <c r="E85" s="6">
         <v>0.72360300256890098</v>
       </c>
-      <c r="F82" s="6">
+      <c r="F85" s="6">
         <v>6.4177281301230002E-2</v>
       </c>
-      <c r="G82" s="6">
+      <c r="G85" s="6">
         <v>0.45731255796516501</v>
       </c>
-      <c r="H82" s="6">
+      <c r="H85" s="6">
         <v>0.105443254817987</v>
       </c>
-      <c r="I82" s="6">
+      <c r="I85" s="6">
         <v>2.0492505353319101E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A83" s="4">
+    <row r="86" spans="1:9">
+      <c r="A86" s="4">
         <v>108</v>
       </c>
-      <c r="B83" s="5">
+      <c r="B86" s="5">
         <v>24386.0085801368</v>
       </c>
-      <c r="C83" s="6">
+      <c r="C86" s="6">
         <v>0.35311776396202799</v>
       </c>
-      <c r="D83" s="6">
+      <c r="D86" s="6">
         <v>9.8039373455680798E-2</v>
       </c>
-      <c r="E83" s="6">
+      <c r="E86" s="6">
         <v>0.76954164718622298</v>
       </c>
-      <c r="F83" s="6">
+      <c r="F86" s="6">
         <v>4.0967976690395098E-2</v>
       </c>
-      <c r="G83" s="6">
+      <c r="G86" s="6">
         <v>0.42008476929259803</v>
       </c>
-      <c r="H83" s="6">
+      <c r="H86" s="6">
         <v>0.12349864807172301</v>
       </c>
-      <c r="I83" s="6">
+      <c r="I86" s="6">
         <v>2.3523552013661599E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A84" s="4">
+    <row r="87" spans="1:9">
+      <c r="A87" s="4">
         <v>109</v>
       </c>
-      <c r="B84" s="5">
+      <c r="B87" s="5">
         <v>26522.0852844537</v>
       </c>
-      <c r="C84" s="6">
+      <c r="C87" s="6">
         <v>0.36735714458295898</v>
       </c>
-      <c r="D84" s="6">
+      <c r="D87" s="6">
         <v>0.164400468268007</v>
       </c>
-      <c r="E84" s="6">
+      <c r="E87" s="6">
         <v>0.73181348488766296</v>
       </c>
-      <c r="F84" s="6">
+      <c r="F87" s="6">
         <v>7.08457203778943E-2</v>
       </c>
-      <c r="G84" s="6">
+      <c r="G87" s="6">
         <v>0.45488536501605598</v>
       </c>
-      <c r="H84" s="6">
+      <c r="H87" s="6">
         <v>7.8138385502471194E-2</v>
       </c>
-      <c r="I84" s="6">
+      <c r="I87" s="6">
         <v>2.0115321252059299E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A85" s="4">
+    <row r="88" spans="1:9">
+      <c r="A88" s="4">
         <v>110</v>
       </c>
-      <c r="B85" s="5">
+      <c r="B88" s="5">
         <v>27024.797975234698</v>
       </c>
-      <c r="C85" s="6">
+      <c r="C88" s="6">
         <v>0.35479211726549997</v>
       </c>
-      <c r="D85" s="6">
+      <c r="D88" s="6">
         <v>0.14426013464543</v>
       </c>
-      <c r="E85" s="6">
+      <c r="E88" s="6">
         <v>0.76471678178820601</v>
       </c>
-      <c r="F85" s="6">
+      <c r="F88" s="6">
         <v>5.6696011100946901E-2</v>
       </c>
-      <c r="G85" s="6">
+      <c r="G88" s="6">
         <v>0.43805415776995199</v>
       </c>
-      <c r="H85" s="6">
+      <c r="H88" s="6">
         <v>9.2954475069681006E-2</v>
       </c>
-      <c r="I85" s="6">
+      <c r="I88" s="6">
         <v>1.8321461752864698E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A86" s="4">
+    <row r="89" spans="1:9">
+      <c r="A89" s="4">
         <v>111</v>
       </c>
-      <c r="B86" s="5">
+      <c r="B89" s="5">
         <v>27094.0520626941</v>
       </c>
-      <c r="C86" s="6">
+      <c r="C89" s="6">
         <v>0.36163844813503498</v>
       </c>
-      <c r="D86" s="6">
+      <c r="D89" s="6">
         <v>0.16153079764849501</v>
       </c>
-      <c r="E86" s="6">
+      <c r="E89" s="6">
         <v>0.73731515082620802</v>
       </c>
-      <c r="F86" s="6">
+      <c r="F89" s="6">
         <v>6.8550923911450498E-2</v>
       </c>
-      <c r="G86" s="6">
+      <c r="G89" s="6">
         <v>0.44498301371938398</v>
       </c>
-      <c r="H86" s="6">
+      <c r="H89" s="6">
         <v>7.0585620915032704E-2</v>
       </c>
-      <c r="I86" s="6">
+      <c r="I89" s="6">
         <v>1.5845751633986899E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A87" s="4">
+    <row r="90" spans="1:9">
+      <c r="A90" s="4">
         <v>112</v>
       </c>
-      <c r="B87" s="5">
+      <c r="B90" s="5">
         <v>27848.273335375499</v>
       </c>
-      <c r="C87" s="6">
+      <c r="C90" s="6">
         <v>0.35247350393524601</v>
       </c>
-      <c r="D87" s="6">
+      <c r="D90" s="6">
         <v>0.18284761430495999</v>
       </c>
-      <c r="E87" s="6">
+      <c r="E90" s="6">
         <v>0.72167224019302401</v>
       </c>
-      <c r="F87" s="6">
+      <c r="F90" s="6">
         <v>6.4226088487186597E-2</v>
       </c>
-      <c r="G87" s="6">
+      <c r="G90" s="6">
         <v>0.42549967112578602</v>
       </c>
-      <c r="H87" s="6">
+      <c r="H90" s="6">
         <v>7.4430864647938702E-2</v>
       </c>
-      <c r="I87" s="6">
+      <c r="I90" s="6">
         <v>1.1743889091572399E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A88" s="4">
+    <row r="91" spans="1:9">
+      <c r="A91" s="4">
         <v>113</v>
       </c>
-      <c r="B88" s="5">
+      <c r="B91" s="5">
         <v>26129.4539415334</v>
       </c>
-      <c r="C88" s="6">
+      <c r="C91" s="6">
         <v>0.36752135130064101</v>
       </c>
-      <c r="D88" s="6">
+      <c r="D91" s="6">
         <v>0.15080490881157499</v>
       </c>
-      <c r="E88" s="6">
+      <c r="E91" s="6">
         <v>0.74774100578886304</v>
       </c>
-      <c r="F88" s="6">
+      <c r="F91" s="6">
         <v>6.2942674687299194E-2</v>
       </c>
-      <c r="G88" s="6">
+      <c r="G91" s="6">
         <v>0.45430268946357599</v>
       </c>
-      <c r="H88" s="6">
+      <c r="H91" s="6">
         <v>0.12727548111190301</v>
       </c>
-      <c r="I88" s="6">
+      <c r="I91" s="6">
         <v>2.54550962223806E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A89" s="4">
+    <row r="92" spans="1:9">
+      <c r="A92" s="4">
         <v>114</v>
       </c>
-      <c r="B89" s="5">
+      <c r="B92" s="5">
         <v>26063.4319155132</v>
       </c>
-      <c r="C89" s="6">
+      <c r="C92" s="6">
         <v>0.37980546409791399</v>
       </c>
-      <c r="D89" s="6">
+      <c r="D92" s="6">
         <v>0.13679540044344099</v>
       </c>
-      <c r="E89" s="6">
+      <c r="E92" s="6">
         <v>0.77813910442674705</v>
       </c>
-      <c r="F89" s="6">
+      <c r="F92" s="6">
         <v>5.2913329626509097E-2</v>
       </c>
-      <c r="G89" s="6">
+      <c r="G92" s="6">
         <v>0.47046359484026601</v>
       </c>
-      <c r="H89" s="6">
+      <c r="H92" s="6">
         <v>8.5769395627946804E-2</v>
       </c>
-      <c r="I89" s="6">
+      <c r="I92" s="6">
         <v>3.5612944706386603E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A90" s="4">
+    <row r="93" spans="1:9">
+      <c r="A93" s="4">
         <v>115</v>
       </c>
-      <c r="B90" s="5">
+      <c r="B93" s="5">
         <v>22446.7265861173</v>
       </c>
-      <c r="C90" s="6">
+      <c r="C93" s="6">
         <v>0.30928813539417999</v>
       </c>
-      <c r="D90" s="6">
+      <c r="D93" s="6">
         <v>0.109356672417732</v>
       </c>
-      <c r="E90" s="6">
+      <c r="E93" s="6">
         <v>0.66953903293415995</v>
       </c>
-      <c r="F90" s="6">
+      <c r="F93" s="6">
         <v>4.6043621554226498E-2</v>
       </c>
-      <c r="G90" s="6">
+      <c r="G93" s="6">
         <v>0.373695520452901</v>
       </c>
-      <c r="H90" s="6">
+      <c r="H93" s="6">
         <v>0.10722745008033099</v>
       </c>
-      <c r="I90" s="6">
+      <c r="I93" s="6">
         <v>1.6173972917144799E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A91" s="4">
+    <row r="94" spans="1:9">
+      <c r="A94" s="4">
         <v>117</v>
       </c>
-      <c r="B91" s="5">
+      <c r="B94" s="5">
         <v>26620.887167343099</v>
       </c>
-      <c r="C91" s="6">
+      <c r="C94" s="6">
         <v>0.349178912879125</v>
       </c>
-      <c r="D91" s="6">
+      <c r="D94" s="6">
         <v>0.202895871126445</v>
       </c>
-      <c r="E91" s="6">
+      <c r="E94" s="6">
         <v>0.661737886968779</v>
       </c>
-      <c r="F91" s="6">
+      <c r="F94" s="6">
         <v>8.2241184992090294E-2</v>
       </c>
-      <c r="G91" s="6">
+      <c r="G94" s="6">
         <v>0.432810605146906</v>
       </c>
-      <c r="H91" s="6">
+      <c r="H94" s="6">
         <v>7.9176598049837496E-2</v>
       </c>
-      <c r="I91" s="6">
+      <c r="I94" s="6">
         <v>3.3618634886240499E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A92" s="4">
+    <row r="95" spans="1:9">
+      <c r="A95" s="4">
         <v>118</v>
       </c>
-      <c r="B92" s="5">
+      <c r="B95" s="5">
         <v>26178.102630217301</v>
       </c>
-      <c r="C92" s="6">
+      <c r="C95" s="6">
         <v>0.345476557431942</v>
       </c>
-      <c r="D92" s="6">
+      <c r="D95" s="6">
         <v>0.172367595629521</v>
       </c>
-      <c r="E92" s="6">
+      <c r="E95" s="6">
         <v>0.71870104753640696</v>
       </c>
-      <c r="F92" s="6">
+      <c r="F95" s="6">
         <v>7.5915514145093205E-2</v>
       </c>
-      <c r="G92" s="6">
+      <c r="G95" s="6">
         <v>0.413360791708271</v>
       </c>
-      <c r="H92" s="6">
+      <c r="H95" s="6">
         <v>8.9452736318407999E-2</v>
       </c>
-      <c r="I92" s="6">
+      <c r="I95" s="6">
         <v>1.2985074626865699E-2</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A93" s="4">
+    <row r="96" spans="1:9">
+      <c r="A96" s="4">
         <v>119</v>
       </c>
-      <c r="B93" s="5">
+      <c r="B96" s="5">
         <v>25345.6793653352</v>
       </c>
-      <c r="C93" s="6">
+      <c r="C96" s="6">
         <v>0.35483589044012198</v>
       </c>
-      <c r="D93" s="6">
+      <c r="D96" s="6">
         <v>0.13768777779435801</v>
       </c>
-      <c r="E93" s="6">
+      <c r="E96" s="6">
         <v>0.77240271213299405</v>
       </c>
-      <c r="F93" s="6">
+      <c r="F96" s="6">
         <v>5.7388426941741101E-2</v>
       </c>
-      <c r="G93" s="6">
+      <c r="G96" s="6">
         <v>0.45636479609995301</v>
       </c>
-      <c r="H93" s="6">
+      <c r="H96" s="6">
         <v>0.10431654676259</v>
       </c>
-      <c r="I93" s="6">
+      <c r="I96" s="6">
         <v>8.3453237410071896E-3</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A94" s="4">
+    <row r="97" spans="1:9">
+      <c r="A97" s="4">
         <v>120</v>
       </c>
-      <c r="B94" s="5">
+      <c r="B97" s="5">
         <v>27380.544568221099</v>
       </c>
-      <c r="C94" s="6">
+      <c r="C97" s="6">
         <v>0.35992780895570903</v>
       </c>
-      <c r="D94" s="6">
+      <c r="D97" s="6">
         <v>0.188681952361373</v>
       </c>
-      <c r="E94" s="6">
+      <c r="E97" s="6">
         <v>0.70409229619444103</v>
       </c>
-      <c r="F94" s="6">
+      <c r="F97" s="6">
         <v>7.7999728573571903E-2</v>
       </c>
-      <c r="G94" s="6">
+      <c r="G97" s="6">
         <v>0.44585530158071501</v>
       </c>
-      <c r="H94" s="6">
+      <c r="H97" s="6">
         <v>6.0737802459341503E-2</v>
       </c>
-      <c r="I94" s="6">
+      <c r="I97" s="6">
         <v>1.13883379611265E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A95" s="4">
+    <row r="98" spans="1:9">
+      <c r="A98" s="4">
         <v>123</v>
       </c>
-      <c r="B95" s="5">
+      <c r="B98" s="5">
         <v>26632.279927964501</v>
       </c>
-      <c r="C95" s="6">
+      <c r="C98" s="6">
         <v>0.36612246925471598</v>
       </c>
-      <c r="D95" s="6">
+      <c r="D98" s="6">
         <v>0.13285642463043301</v>
       </c>
-      <c r="E95" s="6">
+      <c r="E98" s="6">
         <v>0.79069409137681601</v>
       </c>
-      <c r="F95" s="6">
+      <c r="F98" s="6">
         <v>5.6063016068012603E-2</v>
       </c>
-      <c r="G95" s="6">
+      <c r="G98" s="6">
         <v>0.45031350426206801</v>
       </c>
-      <c r="H95" s="6">
+      <c r="H98" s="6">
         <v>4.1844868465620397E-2</v>
       </c>
-      <c r="I95" s="6">
+      <c r="I98" s="6">
         <v>9.1351473410861504E-3</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A96" s="4">
+    <row r="99" spans="1:9">
+      <c r="A99" s="4">
         <v>124</v>
       </c>
-      <c r="B96" s="5">
+      <c r="B99" s="5">
         <v>29573.274763858801</v>
       </c>
-      <c r="C96" s="6">
+      <c r="C99" s="6">
         <v>0.35014896582626798</v>
       </c>
-      <c r="D96" s="6">
+      <c r="D99" s="6">
         <v>0.24961616172065201</v>
       </c>
-      <c r="E96" s="6">
+      <c r="E99" s="6">
         <v>0.62487518259594099</v>
       </c>
-      <c r="F96" s="6">
+      <c r="F99" s="6">
         <v>9.1612728276907002E-2</v>
       </c>
-      <c r="G96" s="6">
+      <c r="G99" s="6">
         <v>0.42810868913109901</v>
       </c>
-      <c r="H96" s="6">
+      <c r="H99" s="6">
         <v>5.9628684149454603E-2</v>
       </c>
-      <c r="I96" s="6">
+      <c r="I99" s="6">
         <v>7.7396147598050597E-3</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A97" s="4">
+    <row r="100" spans="1:9">
+      <c r="A100" s="4">
         <v>125</v>
       </c>
-      <c r="B97" s="5">
+      <c r="B100" s="5">
         <v>29967.129550096</v>
       </c>
-      <c r="C97" s="6">
+      <c r="C100" s="6">
         <v>0.34111519075396401</v>
       </c>
-      <c r="D97" s="6">
+      <c r="D100" s="6">
         <v>0.25965840628770298</v>
       </c>
-      <c r="E97" s="6">
+      <c r="E100" s="6">
         <v>0.62029108789269405</v>
       </c>
-      <c r="F97" s="6">
+      <c r="F100" s="6">
         <v>8.6622919162644099E-2</v>
       </c>
-      <c r="G97" s="6">
+      <c r="G100" s="6">
         <v>0.42379519169386398</v>
       </c>
-      <c r="H97" s="6">
+      <c r="H100" s="6">
         <v>5.5459598526235498E-2</v>
       </c>
-      <c r="I97" s="6">
+      <c r="I100" s="6">
         <v>9.5334137974844406E-3</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A98" s="4">
+    <row r="101" spans="1:9">
+      <c r="A101" s="4">
         <v>126</v>
       </c>
-      <c r="B98" s="5">
+      <c r="B101" s="5">
         <v>27411.568354732099</v>
       </c>
-      <c r="C98" s="6">
+      <c r="C101" s="6">
         <v>0.34454113553653698</v>
       </c>
-      <c r="D98" s="6">
+      <c r="D101" s="6">
         <v>0.17625097980749099</v>
       </c>
-      <c r="E98" s="6">
+      <c r="E101" s="6">
         <v>0.73137657880041096</v>
       </c>
-      <c r="F98" s="6">
+      <c r="F101" s="6">
         <v>6.0901369363012298E-2</v>
       </c>
-      <c r="G98" s="6">
+      <c r="G101" s="6">
         <v>0.41853547168018201</v>
       </c>
-      <c r="H98" s="6">
+      <c r="H101" s="6">
         <v>6.1640354254909498E-2</v>
       </c>
-      <c r="I98" s="6">
+      <c r="I101" s="6">
         <v>2.0435117443203699E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A99" s="4">
+    <row r="102" spans="1:9">
+      <c r="A102" s="4">
         <v>127</v>
       </c>
-      <c r="B99" s="5">
+      <c r="B102" s="5">
         <v>30185.7127515879</v>
       </c>
-      <c r="C99" s="6">
+      <c r="C102" s="6">
         <v>0.306684455096222</v>
       </c>
-      <c r="D99" s="6">
+      <c r="D102" s="6">
         <v>0.35262520510468898</v>
       </c>
-      <c r="E99" s="6">
+      <c r="E102" s="6">
         <v>0.45538685535273399</v>
       </c>
-      <c r="F99" s="6">
+      <c r="F102" s="6">
         <v>0.135344503779809</v>
       </c>
-      <c r="G99" s="6">
+      <c r="G102" s="6">
         <v>0.34947993933440202</v>
       </c>
-      <c r="H99" s="6">
+      <c r="H102" s="6">
         <v>0.15669793621013101</v>
       </c>
-      <c r="I99" s="6">
+      <c r="I102" s="6">
         <v>4.4071294559099403E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A100" s="4">
+    <row r="103" spans="1:9">
+      <c r="A103" s="4">
         <v>128</v>
       </c>
-      <c r="B100" s="5">
+      <c r="B103" s="5">
         <v>30669.3675196402</v>
       </c>
-      <c r="C100" s="6">
+      <c r="C103" s="6">
         <v>0.263969364651159</v>
       </c>
-      <c r="D100" s="6">
+      <c r="D103" s="6">
         <v>0.47014718692044699</v>
       </c>
-      <c r="E100" s="6">
+      <c r="E103" s="6">
         <v>0.30981372084567599</v>
       </c>
-      <c r="F100" s="6">
+      <c r="F103" s="6">
         <v>0.14654069658676699</v>
       </c>
-      <c r="G100" s="6">
+      <c r="G103" s="6">
         <v>0.26390900020649999</v>
       </c>
-      <c r="H100" s="6">
+      <c r="H103" s="6">
         <v>0.221540983606557</v>
       </c>
-      <c r="I100" s="6">
+      <c r="I103" s="6">
         <v>1.7114754098360701E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A101" s="4">
+    <row r="104" spans="1:9">
+      <c r="A104" s="4">
         <v>129</v>
       </c>
-      <c r="B101" s="5">
+      <c r="B104" s="5">
         <v>35886.9349794808</v>
       </c>
-      <c r="C101" s="6">
+      <c r="C104" s="6">
         <v>0.20470794591981401</v>
       </c>
-      <c r="D101" s="6">
+      <c r="D104" s="6">
         <v>0.56771647004024195</v>
       </c>
-      <c r="E101" s="6">
+      <c r="E104" s="6">
         <v>0.218379918134502</v>
       </c>
-      <c r="F101" s="6">
+      <c r="F104" s="6">
         <v>0.140630695483975</v>
       </c>
-      <c r="G101" s="6">
+      <c r="G104" s="6">
         <v>0.19930421775924501</v>
       </c>
-      <c r="H101" s="6">
+      <c r="H104" s="6">
         <v>8.6945403200501994E-2</v>
       </c>
-      <c r="I101" s="6">
+      <c r="I104" s="6">
         <v>2.5933479761531202E-2</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A102" s="4">
+    <row r="105" spans="1:9">
+      <c r="A105" s="4">
         <v>130</v>
       </c>
-      <c r="B102" s="5">
+      <c r="B105" s="5">
         <v>33738.433588312102</v>
       </c>
-      <c r="C102" s="6">
+      <c r="C105" s="6">
         <v>0.22274532261899699</v>
       </c>
-      <c r="D102" s="6">
+      <c r="D105" s="6">
         <v>0.55663750918479205</v>
       </c>
-      <c r="E102" s="6">
+      <c r="E105" s="6">
         <v>0.231150949159735</v>
       </c>
-      <c r="F102" s="6">
+      <c r="F105" s="6">
         <v>0.13440959471734501</v>
       </c>
-      <c r="G102" s="6">
+      <c r="G105" s="6">
         <v>0.20766323576318099</v>
       </c>
-      <c r="H102" s="6">
+      <c r="H105" s="6">
         <v>0.21318238213399501</v>
       </c>
-      <c r="I102" s="6">
+      <c r="I105" s="6">
         <v>2.4466501240694799E-2</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A103" s="4">
+    <row r="106" spans="1:9">
+      <c r="A106" s="4">
         <v>131</v>
       </c>
-      <c r="B103" s="5">
+      <c r="B106" s="5">
         <v>27383.748940331399</v>
       </c>
-      <c r="C103" s="6">
+      <c r="C106" s="6">
         <v>0.35691020718922001</v>
       </c>
-      <c r="D103" s="6">
+      <c r="D106" s="6">
         <v>0.195109825671056</v>
       </c>
-      <c r="E103" s="6">
+      <c r="E106" s="6">
         <v>0.70402948793041598</v>
       </c>
-      <c r="F103" s="6">
+      <c r="F106" s="6">
         <v>7.1835887708891294E-2</v>
       </c>
-      <c r="G103" s="6">
+      <c r="G106" s="6">
         <v>0.43332923108068</v>
       </c>
-      <c r="H103" s="6">
+      <c r="H106" s="6">
         <v>3.4261061946902698E-2</v>
       </c>
-      <c r="I103" s="6">
+      <c r="I106" s="6">
         <v>1.5013274336283199E-2</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A104" s="4">
+    <row r="107" spans="1:9">
+      <c r="A107" s="4">
         <v>132</v>
       </c>
-      <c r="B104" s="5">
+      <c r="B107" s="5">
         <v>27450.683717398799</v>
       </c>
-      <c r="C104" s="6">
+      <c r="C107" s="6">
         <v>0.364658632813396</v>
       </c>
-      <c r="D104" s="6">
+      <c r="D107" s="6">
         <v>0.24828362252126801</v>
       </c>
-      <c r="E104" s="6">
+      <c r="E107" s="6">
         <v>0.58872040583246499</v>
       </c>
-      <c r="F104" s="6">
+      <c r="F107" s="6">
         <v>0.128603933697437</v>
       </c>
-      <c r="G104" s="6">
+      <c r="G107" s="6">
         <v>0.426232648921127</v>
       </c>
-      <c r="H104" s="6">
+      <c r="H107" s="6">
         <v>0.219742268041237</v>
       </c>
-      <c r="I104" s="6">
+      <c r="I107" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A105" s="4">
+    <row r="108" spans="1:9">
+      <c r="A108" s="4">
         <v>133</v>
       </c>
-      <c r="B105" s="5">
+      <c r="B108" s="5">
         <v>36307.284747069803</v>
       </c>
-      <c r="C105" s="6">
+      <c r="C108" s="6">
         <v>0.21198327183069701</v>
       </c>
-      <c r="D105" s="6">
+      <c r="D108" s="6">
         <v>0.50972514032348304</v>
       </c>
-      <c r="E105" s="6">
+      <c r="E108" s="6">
         <v>0.29075669183351599</v>
       </c>
-      <c r="F105" s="6">
+      <c r="F108" s="6">
         <v>0.12980173775918999</v>
       </c>
-      <c r="G105" s="6">
+      <c r="G108" s="6">
         <v>0.23029471357342099</v>
       </c>
-      <c r="H105" s="6">
+      <c r="H108" s="6">
         <v>1.5703971119133599E-2</v>
       </c>
-      <c r="I105" s="6">
+      <c r="I108" s="6">
         <v>4.7111913357400703E-3</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A106" s="4">
+    <row r="109" spans="1:9">
+      <c r="A109" s="4">
         <v>139</v>
       </c>
-      <c r="B106" s="5">
+      <c r="B109" s="5">
         <v>29834.012834568501</v>
       </c>
-      <c r="C106" s="6">
+      <c r="C109" s="6">
         <v>0.35984570721936798</v>
       </c>
-      <c r="D106" s="6">
+      <c r="D109" s="6">
         <v>0.22813933521181301</v>
       </c>
-      <c r="E106" s="6">
+      <c r="E109" s="6">
         <v>0.67192911664419397</v>
       </c>
-      <c r="F106" s="6">
+      <c r="F109" s="6">
         <v>7.3664056418791396E-2</v>
       </c>
-      <c r="G106" s="6">
+      <c r="G109" s="6">
         <v>0.43491330035597298</v>
       </c>
-      <c r="H106" s="6">
+      <c r="H109" s="6">
         <v>6.5283307810107202E-2</v>
       </c>
-      <c r="I106" s="6">
+      <c r="I109" s="6">
         <v>0.17719754977029101</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A107" s="4">
+    <row r="110" spans="1:9">
+      <c r="A110" s="4">
         <v>150</v>
       </c>
-      <c r="B107" s="5">
+      <c r="B110" s="5">
         <v>37117.375570108503</v>
       </c>
-      <c r="C107" s="6">
+      <c r="C110" s="6">
         <v>0.21412461170449601</v>
       </c>
-      <c r="D107" s="6">
+      <c r="D110" s="6">
         <v>0.47390333875235902</v>
       </c>
-      <c r="E107" s="6">
+      <c r="E110" s="6">
         <v>0.39598267410856702</v>
       </c>
-      <c r="F107" s="6">
+      <c r="F110" s="6">
         <v>8.4945024004647499E-2</v>
       </c>
-      <c r="G107" s="6">
+      <c r="G110" s="6">
         <v>0.22485455900509899</v>
       </c>
-      <c r="H107" s="6">
+      <c r="H110" s="6">
         <v>0.393287671232877</v>
       </c>
-      <c r="I107" s="6">
+      <c r="I110" s="6">
         <v>1.78767123287671E-2</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A108" s="4">
+    <row r="111" spans="1:9">
+      <c r="A111" s="4">
         <v>201</v>
       </c>
-      <c r="B108" s="5">
+      <c r="B111" s="5">
         <v>27819.793071050699</v>
       </c>
-      <c r="C108" s="6">
+      <c r="C111" s="6">
         <v>0.36326848785867899</v>
       </c>
-      <c r="D108" s="6">
+      <c r="D111" s="6">
         <v>0.23987327249002499</v>
       </c>
-      <c r="E108" s="6">
+      <c r="E111" s="6">
         <v>0.57482467043351004</v>
       </c>
-      <c r="F108" s="6">
+      <c r="F111" s="6">
         <v>0.14919013198921799</v>
       </c>
-      <c r="G108" s="6">
+      <c r="G111" s="6">
         <v>0.44077164609602298</v>
       </c>
-      <c r="H108" s="6">
+      <c r="H111" s="6">
         <v>5.2590673575129499E-3</v>
       </c>
-      <c r="I108" s="6">
+      <c r="I111" s="6">
         <v>2.25388601036269E-3</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A109" s="4">
+    <row r="112" spans="1:9">
+      <c r="A112" s="4">
         <v>204</v>
       </c>
-      <c r="B109" s="5">
+      <c r="B112" s="5">
         <v>24976.101908160301</v>
       </c>
-      <c r="C109" s="6">
+      <c r="C112" s="6">
         <v>0.39591503312264897</v>
       </c>
-      <c r="D109" s="6">
+      <c r="D112" s="6">
         <v>0.162661506572189</v>
       </c>
-      <c r="E109" s="6">
+      <c r="E112" s="6">
         <v>0.70065140919403202</v>
       </c>
-      <c r="F109" s="6">
+      <c r="F112" s="6">
         <v>0.101110075304109</v>
       </c>
-      <c r="G109" s="6">
+      <c r="G112" s="6">
         <v>0.46288592982500498</v>
       </c>
-      <c r="H109" s="6">
+      <c r="H112" s="6">
         <v>6.8138479001135094E-2</v>
       </c>
-      <c r="I109" s="6">
+      <c r="I112" s="6">
         <v>2.96254256526674E-3</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A110" s="4">
+    <row r="113" spans="1:9">
+      <c r="A113" s="4">
         <v>206</v>
       </c>
-      <c r="B110" s="5">
+      <c r="B113" s="5">
         <v>25271.725306246499</v>
       </c>
-      <c r="C110" s="6">
+      <c r="C113" s="6">
         <v>0.39591229901825897</v>
       </c>
-      <c r="D110" s="6">
+      <c r="D113" s="6">
         <v>0.24392302480925501</v>
       </c>
-      <c r="E110" s="6">
+      <c r="E113" s="6">
         <v>0.58588105078230002</v>
       </c>
-      <c r="F110" s="6">
+      <c r="F113" s="6">
         <v>0.13167079290134101</v>
       </c>
-      <c r="G110" s="6">
+      <c r="G113" s="6">
         <v>0.495617482293293</v>
       </c>
-      <c r="H110" s="6">
+      <c r="H113" s="6">
         <v>6.9802325581395305E-2</v>
       </c>
-      <c r="I110" s="6">
+      <c r="I113" s="6">
         <v>1.01162790697674E-3</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A111" s="4">
+    <row r="114" spans="1:9">
+      <c r="A114" s="4">
         <v>310</v>
       </c>
-      <c r="B111" s="5">
+      <c r="B114" s="5">
         <v>29121.5844417564</v>
       </c>
-      <c r="C111" s="6">
+      <c r="C114" s="6">
         <v>0.31969624090284798</v>
       </c>
-      <c r="D111" s="6">
+      <c r="D114" s="6">
         <v>0.15988042089288501</v>
       </c>
-      <c r="E111" s="6">
+      <c r="E114" s="6">
         <v>0.72175703014410797</v>
       </c>
-      <c r="F111" s="6">
+      <c r="F114" s="6">
         <v>8.5985918707425293E-2</v>
       </c>
-      <c r="G111" s="6">
+      <c r="G114" s="6">
         <v>0.37904922707654198</v>
       </c>
-      <c r="H111" s="6">
+      <c r="H114" s="6">
         <v>1.90260294431406E-2</v>
       </c>
-      <c r="I111" s="6">
+      <c r="I114" s="6">
         <v>5.8470236825261396E-3</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A112" s="4">
+    <row r="115" spans="1:9">
+      <c r="A115" s="4">
         <v>311</v>
       </c>
-      <c r="B112" s="5">
+      <c r="B115" s="5">
         <v>28318.8240700889</v>
       </c>
-      <c r="C112" s="6">
+      <c r="C115" s="6">
         <v>0.32289889132594202</v>
       </c>
-      <c r="D112" s="6">
+      <c r="D115" s="6">
         <v>0.16127600950703599</v>
       </c>
-      <c r="E112" s="6">
+      <c r="E115" s="6">
         <v>0.72339848660081996</v>
       </c>
-      <c r="F112" s="6">
+      <c r="F115" s="6">
         <v>8.2854931501995299E-2</v>
       </c>
-      <c r="G112" s="6">
+      <c r="G115" s="6">
         <v>0.38831496258185699</v>
       </c>
-      <c r="H112" s="6">
+      <c r="H115" s="6">
         <v>3.1979065238558903E-2</v>
       </c>
-      <c r="I112" s="6">
+      <c r="I115" s="6">
         <v>5.71811100292113E-3</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A113" s="4">
+    <row r="116" spans="1:9">
+      <c r="A116" s="4">
         <v>316</v>
       </c>
-      <c r="B113" s="5">
+      <c r="B116" s="5">
         <v>29736.101974974899</v>
       </c>
-      <c r="C113" s="6">
+      <c r="C116" s="6">
         <v>0.31327626065561798</v>
       </c>
-      <c r="D113" s="6">
+      <c r="D116" s="6">
         <v>0.41289164019429098</v>
       </c>
-      <c r="E113" s="6">
+      <c r="E116" s="6">
         <v>0.41823239161015802</v>
       </c>
-      <c r="F113" s="6">
+      <c r="F116" s="6">
         <v>8.7295597188717697E-2</v>
       </c>
-      <c r="G113" s="6">
+      <c r="G116" s="6">
         <v>0.387725820166266</v>
       </c>
-      <c r="H113" s="6">
+      <c r="H116" s="6">
         <v>0.25743164062500001</v>
       </c>
-      <c r="I113" s="6">
+      <c r="I116" s="6">
         <v>2.1240234375E-2</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A114" s="4">
+    <row r="117" spans="1:9">
+      <c r="A117" s="4">
         <v>452</v>
       </c>
-      <c r="B114" s="5">
+      <c r="B117" s="5">
         <v>33908.032648993802</v>
       </c>
-      <c r="C114" s="6">
+      <c r="C117" s="6">
         <v>0.18939396559452301</v>
       </c>
-      <c r="D114" s="6">
+      <c r="D117" s="6">
         <v>0.55526842072224403</v>
       </c>
-      <c r="E114" s="6">
+      <c r="E117" s="6">
         <v>0.19318332146221801</v>
       </c>
-      <c r="F114" s="6">
+      <c r="F117" s="6">
         <v>9.9516818937204599E-2</v>
       </c>
-      <c r="G114" s="6">
+      <c r="G117" s="6">
         <v>0.187570291850093</v>
       </c>
-      <c r="H114" s="6">
+      <c r="H117" s="6">
         <v>6.6923076923076905E-2</v>
       </c>
-      <c r="I114" s="6">
+      <c r="I117" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A115" s="4" t="s">
+    <row r="118" spans="1:9">
+      <c r="A118" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B115" s="5">
+      <c r="B118" s="5">
         <v>27142.9535276487</v>
       </c>
-      <c r="C115" s="6">
+      <c r="C118" s="6">
         <v>0.296137446953459</v>
       </c>
-      <c r="D115" s="6">
+      <c r="D118" s="6">
         <v>0.39756525501301399</v>
       </c>
-      <c r="E115" s="6">
+      <c r="E118" s="6">
         <v>0.37637036838489701</v>
       </c>
-      <c r="F115" s="6">
+      <c r="F118" s="6">
         <v>0.14762663357029901</v>
       </c>
-      <c r="G115" s="6">
+      <c r="G118" s="6">
         <v>0.30478511553495402</v>
       </c>
-      <c r="H115" s="6">
+      <c r="H118" s="6">
         <v>8.7781408938426606E-2</v>
       </c>
-      <c r="I115" s="6">
+      <c r="I118" s="6">
         <v>1.47243804783032E-2</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A116" s="4" t="s">
+    <row r="119" spans="1:9">
+      <c r="A119" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B116" s="5">
+      <c r="B119" s="5">
         <v>27845.869488574899</v>
       </c>
-      <c r="C116" s="6">
+      <c r="C119" s="6">
         <v>0.35201557264011002</v>
       </c>
-      <c r="D116" s="6">
+      <c r="D119" s="6">
         <v>0.254948268151027</v>
       </c>
-      <c r="E116" s="6">
+      <c r="E119" s="6">
         <v>0.60587165083884797</v>
       </c>
-      <c r="F116" s="6">
+      <c r="F119" s="6">
         <v>0.106373018861828</v>
       </c>
-      <c r="G116" s="6">
+      <c r="G119" s="6">
         <v>0.44098732064896801</v>
       </c>
-      <c r="H116" s="6">
+      <c r="H119" s="6">
         <v>6.1809518374800303E-2</v>
       </c>
-      <c r="I116" s="6">
+      <c r="I119" s="6">
         <v>1.16172106824926E-2</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A117" s="4" t="s">
+    <row r="120" spans="1:9">
+      <c r="A120" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B117" s="5">
+      <c r="B120" s="5">
         <v>27105.101821571599</v>
       </c>
-      <c r="C117" s="6">
+      <c r="C120" s="6">
         <v>0.35611045740302799</v>
       </c>
-      <c r="D117" s="6">
+      <c r="D120" s="6">
         <v>0.17203762577849599</v>
       </c>
-      <c r="E117" s="6">
+      <c r="E120" s="6">
         <v>0.74627473294816105</v>
       </c>
-      <c r="F117" s="6">
+      <c r="F120" s="6">
         <v>4.9412513747549298E-2</v>
       </c>
-      <c r="G117" s="6">
+      <c r="G120" s="6">
         <v>0.45021640062600299</v>
       </c>
-      <c r="H117" s="6">
+      <c r="H120" s="6">
         <v>0.16354227382769701</v>
       </c>
-      <c r="I117" s="6">
+      <c r="I120" s="6">
         <v>2.4661917318160101E-2</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A118" s="4" t="s">
+    <row r="121" spans="1:9">
+      <c r="A121" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B118" s="5">
+      <c r="B121" s="5">
         <v>33790.195675110801</v>
       </c>
-      <c r="C118" s="6">
+      <c r="C121" s="6">
         <v>0.28334603134425401</v>
       </c>
-      <c r="D118" s="6">
+      <c r="D121" s="6">
         <v>0.20575909715931001</v>
       </c>
-      <c r="E118" s="6">
+      <c r="E121" s="6">
         <v>0.70966267895840096</v>
       </c>
-      <c r="F118" s="6">
+      <c r="F121" s="6">
         <v>6.0000039529991299E-2</v>
       </c>
-      <c r="G118" s="6">
+      <c r="G121" s="6">
         <v>0.367422081511524</v>
       </c>
-      <c r="H118" s="6">
+      <c r="H121" s="6">
         <v>0.19268277280600499</v>
       </c>
-      <c r="I118" s="6">
+      <c r="I121" s="6">
         <v>3.0876335161662799E-2</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A119" s="4" t="s">
+    <row r="122" spans="1:9">
+      <c r="A122" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B119" s="5">
+      <c r="B122" s="5">
         <v>31897.2077597522</v>
       </c>
-      <c r="C119" s="6">
+      <c r="C122" s="6">
         <v>0.29055899662668799</v>
       </c>
-      <c r="D119" s="6">
+      <c r="D122" s="6">
         <v>0.169742120228281</v>
       </c>
-      <c r="E119" s="6">
+      <c r="E122" s="6">
         <v>0.756355043203219</v>
       </c>
-      <c r="F119" s="6">
+      <c r="F122" s="6">
         <v>5.3935591549090701E-2</v>
       </c>
-      <c r="G119" s="6">
+      <c r="G122" s="6">
         <v>0.36345455877088101</v>
       </c>
-      <c r="H119" s="6">
+      <c r="H122" s="6">
         <v>0.18341770039494901</v>
       </c>
-      <c r="I119" s="6">
+      <c r="I122" s="6">
         <v>2.72464816153975E-2</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A120" s="4" t="s">
+    <row r="123" spans="1:9">
+      <c r="A123" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B120" s="5">
+      <c r="B123" s="5">
         <v>26246.796288266902</v>
       </c>
-      <c r="C120" s="6">
+      <c r="C123" s="6">
         <v>0.35777379854791502</v>
       </c>
-      <c r="D120" s="6">
+      <c r="D123" s="6">
         <v>0.17043101398806701</v>
       </c>
-      <c r="E120" s="6">
+      <c r="E123" s="6">
         <v>0.64302731458555296</v>
       </c>
-      <c r="F120" s="6">
+      <c r="F123" s="6">
         <v>0.15388413448549901</v>
       </c>
-      <c r="G120" s="6">
+      <c r="G123" s="6">
         <v>0.388281361061103</v>
       </c>
-      <c r="H120" s="6">
+      <c r="H123" s="6">
         <v>0.15448371158194499</v>
       </c>
-      <c r="I120" s="6">
+      <c r="I123" s="6">
         <v>2.1978896239845901E-2</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A121" s="4" t="s">
+    <row r="124" spans="1:9">
+      <c r="A124" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B121" s="5">
+      <c r="B124" s="5">
         <v>28843.066977947499</v>
       </c>
-      <c r="C121" s="6">
+      <c r="C124" s="6">
         <v>0.31052669851958697</v>
       </c>
-      <c r="D121" s="6">
+      <c r="D124" s="6">
         <v>0.16043433285515299</v>
       </c>
-      <c r="E121" s="6">
+      <c r="E124" s="6">
         <v>0.70632760556261298</v>
       </c>
-      <c r="F121" s="6">
+      <c r="F124" s="6">
         <v>9.7029037421802397E-2</v>
       </c>
-      <c r="G121" s="6">
+      <c r="G124" s="6">
         <v>0.36405610723494403</v>
       </c>
-      <c r="H121" s="6">
+      <c r="H124" s="6">
         <v>0.15855690528486299</v>
       </c>
-      <c r="I121" s="6">
+      <c r="I124" s="6">
         <v>3.1322963826258501E-2</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A122" s="4" t="s">
+    <row r="125" spans="1:9">
+      <c r="A125" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B122" s="5">
+      <c r="B125" s="5">
         <v>30206.805074667202</v>
       </c>
-      <c r="C122" s="6">
+      <c r="C125" s="6">
         <v>0.27319607236920601</v>
       </c>
-      <c r="D122" s="6">
+      <c r="D125" s="6">
         <v>0.15034121469452399</v>
       </c>
-      <c r="E122" s="6">
+      <c r="E125" s="6">
         <v>0.77662842253729103</v>
       </c>
-      <c r="F122" s="6">
+      <c r="F125" s="6">
         <v>5.16555224088198E-2</v>
       </c>
-      <c r="G122" s="6">
+      <c r="G125" s="6">
         <v>0.35729411916904602</v>
       </c>
-      <c r="H122" s="6">
+      <c r="H125" s="6">
         <v>0.122049734909825</v>
       </c>
-      <c r="I122" s="6">
+      <c r="I125" s="6">
         <v>2.0833758512832999E-2</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A123" s="4" t="s">
+    <row r="126" spans="1:9">
+      <c r="A126" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B123" s="5">
+      <c r="B126" s="5">
         <v>29228.182963775402</v>
       </c>
-      <c r="C123" s="6">
+      <c r="C126" s="6">
         <v>0.33880339361563999</v>
       </c>
-      <c r="D123" s="6">
+      <c r="D126" s="6">
         <v>0.33854063526782202</v>
       </c>
-      <c r="E123" s="6">
+      <c r="E126" s="6">
         <v>0.51472553854723102</v>
       </c>
-      <c r="F123" s="6">
+      <c r="F126" s="6">
         <v>8.1232643541214095E-2</v>
       </c>
-      <c r="G123" s="6">
+      <c r="G126" s="6">
         <v>0.43460256647581103</v>
       </c>
-      <c r="H123" s="6">
+      <c r="H126" s="6">
         <v>0.41682144364710799</v>
       </c>
-      <c r="I123" s="6">
+      <c r="I126" s="6">
         <v>2.4972562262558E-2</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A124" s="4" t="s">
+    <row r="127" spans="1:9">
+      <c r="A127" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B124" s="5">
+      <c r="B127" s="5">
         <v>28534.733806029901</v>
       </c>
-      <c r="C124" s="6">
+      <c r="C127" s="6">
         <v>0.35366319290833398</v>
       </c>
-      <c r="D124" s="6">
+      <c r="D127" s="6">
         <v>0.32987669831887201</v>
       </c>
-      <c r="E124" s="6">
+      <c r="E127" s="6">
         <v>0.528608544236572</v>
       </c>
-      <c r="F124" s="6">
+      <c r="F127" s="6">
         <v>7.9970865115533807E-2</v>
       </c>
-      <c r="G124" s="6">
+      <c r="G127" s="6">
         <v>0.45312682386799802</v>
       </c>
-      <c r="H124" s="6">
+      <c r="H127" s="6">
         <v>0.45871313672922298</v>
       </c>
-      <c r="I124" s="6">
+      <c r="I127" s="6">
         <v>3.0710455764075099E-2</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A125" s="4" t="s">
+    <row r="128" spans="1:9">
+      <c r="A128" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B125" s="5">
+      <c r="B128" s="5">
         <v>27177.994519263699</v>
       </c>
-      <c r="C125" s="6">
+      <c r="C128" s="6">
         <v>0.38198109557683302</v>
       </c>
-      <c r="D125" s="6">
+      <c r="D128" s="6">
         <v>0.26007735670216497</v>
       </c>
-      <c r="E125" s="6">
+      <c r="E128" s="6">
         <v>0.54089969466545296</v>
       </c>
-      <c r="F125" s="6">
+      <c r="F128" s="6">
         <v>0.16226944894169601</v>
       </c>
-      <c r="G125" s="6">
+      <c r="G128" s="6">
         <v>0.44510080175660699</v>
       </c>
-      <c r="H125" s="6">
+      <c r="H128" s="6">
         <v>5.6405195681511498E-2</v>
       </c>
-      <c r="I125" s="6">
+      <c r="I128" s="6">
         <v>9.7840755735492599E-3</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A126" s="4" t="s">
+    <row r="129" spans="1:9">
+      <c r="A129" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B126" s="5">
+      <c r="B129" s="5">
         <v>26100.3989357625</v>
       </c>
-      <c r="C126" s="6">
+      <c r="C129" s="6">
         <v>0.358400687415319</v>
       </c>
-      <c r="D126" s="6">
+      <c r="D129" s="6">
         <v>0.18432854870704601</v>
       </c>
-      <c r="E126" s="6">
+      <c r="E129" s="6">
         <v>0.58538977985343499</v>
       </c>
-      <c r="F126" s="6">
+      <c r="F129" s="6">
         <v>0.18788266096383499</v>
       </c>
-      <c r="G126" s="6">
+      <c r="G129" s="6">
         <v>0.38586501583667598</v>
       </c>
-      <c r="H126" s="6">
+      <c r="H129" s="6">
         <v>0.114879666133316</v>
       </c>
-      <c r="I126" s="6">
+      <c r="I129" s="6">
         <v>2.03353512693202E-2</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A127" s="4" t="s">
+    <row r="130" spans="1:9">
+      <c r="A130" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B127" s="5">
+      <c r="B130" s="5">
         <v>28779.915480427499</v>
       </c>
-      <c r="C127" s="6">
+      <c r="C130" s="6">
         <v>0.33526300217410399</v>
       </c>
-      <c r="D127" s="6">
+      <c r="D130" s="6">
         <v>0.141591944494392</v>
       </c>
-      <c r="E127" s="6">
+      <c r="E130" s="6">
         <v>0.78265851558263999</v>
       </c>
-      <c r="F127" s="6">
+      <c r="F130" s="6">
         <v>5.9599447184197303E-2</v>
       </c>
-      <c r="G127" s="6">
+      <c r="G130" s="6">
         <v>0.39609777133329399</v>
       </c>
-      <c r="H127" s="6">
+      <c r="H130" s="6">
         <v>0.168248275106779</v>
       </c>
-      <c r="I127" s="6">
+      <c r="I130" s="6">
         <v>3.3411455481327401E-2</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I127">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I130">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>